<commit_message>
updated mac version to 0.0.0.0.17
</commit_message>
<xml_diff>
--- a/examples/access.xlsx
+++ b/examples/access.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C2028C-5A0F-7B48-AC22-1A2E2532C9F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1848DA-0A1C-A447-B525-F03AEE946E10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="580" windowWidth="25600" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7700" yWindow="460" windowWidth="25600" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aclrules" sheetId="51" r:id="rId1"/>
@@ -19,8 +19,8 @@
     <sheet name="sshkeys" sheetId="55" r:id="rId4"/>
     <sheet name="vpngateways" sheetId="56" r:id="rId5"/>
     <sheet name="vpnconnections" sheetId="57" r:id="rId6"/>
-    <sheet name="ipsecpolicies" sheetId="58" r:id="rId7"/>
-    <sheet name="ikepolicies" sheetId="59" r:id="rId8"/>
+    <sheet name="ipsecpolicies" sheetId="60" r:id="rId7"/>
+    <sheet name="ikepolicies" sheetId="61" r:id="rId8"/>
     <sheet name="resourcegroups" sheetId="54" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -339,7 +339,6 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -369,7 +368,24 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -503,24 +519,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -681,87 +679,87 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D0CA34BD-A489-B54D-8D4B-B907D54F9FC9}" name="Table3" displayName="Table3" ref="A1:B2" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
-  <autoFilter ref="A1:B2" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D0CA34BD-A489-B54D-8D4B-B907D54F9FC9}" name="Table3" displayName="Table3" ref="A1:B3" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+  <autoFilter ref="A1:B3" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FC67A5D3-A34E-3D4E-9E86-D02090ED17CB}" name="*name" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{F56C754B-0F5D-694F-BD5D-7925CDFC5F97}" name="*public_key" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{FC67A5D3-A34E-3D4E-9E86-D02090ED17CB}" name="*name" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{F56C754B-0F5D-694F-BD5D-7925CDFC5F97}" name="*public_key" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{74F9BE67-E011-B34A-A492-0717499F0410}" name="Table16" displayName="Table16" ref="A1:C2" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A1:C2" xr:uid="{6D379596-E186-C240-BBB4-B8E74F1D3D56}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{74F9BE67-E011-B34A-A492-0717499F0410}" name="Table16" displayName="Table16" ref="A1:C3" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+  <autoFilter ref="A1:C3" xr:uid="{6D379596-E186-C240-BBB4-B8E74F1D3D56}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{5FD29999-A9F5-C549-98A3-DFD2B1437449}" name="*name" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{35CF1270-9B78-4243-98F7-E702702F38FF}" name="*subnet" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{B806F889-718F-584A-ADDF-8A3AD802CDFB}" name="resource_group" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{5FD29999-A9F5-C549-98A3-DFD2B1437449}" name="*name" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{35CF1270-9B78-4243-98F7-E702702F38FF}" name="*subnet" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{B806F889-718F-584A-ADDF-8A3AD802CDFB}" name="resource_group" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B4318CDD-C98E-1341-88CD-5334A857D418}" name="Table15" displayName="Table15" ref="A1:M2" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A1:M2" xr:uid="{27D8B65D-C3AF-BD4B-8BB7-5754C974B57F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B4318CDD-C98E-1341-88CD-5334A857D418}" name="Table15" displayName="Table15" ref="A1:M3" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="A1:M3" xr:uid="{27D8B65D-C3AF-BD4B-8BB7-5754C974B57F}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{C4B8842B-2BB7-EB49-B6D2-B6721C54DC5F}" name="*name" dataDxfId="29"/>
-    <tableColumn id="13" xr3:uid="{78EC6C87-C780-E34D-BBD5-54ED244AB6D6}" name="*vpn_gateway" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{DBBB9AC2-20E7-974C-935D-20C40D819A02}" name="*peer_address" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{5CDA888D-9763-CE46-98E3-D4B85974B5A5}" name="*preshared_key" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{D1C2C80B-E944-E049-AD39-98867623465E}" name="local_cidrs" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{B6F5AA94-6774-DA4F-8D22-7820C9CFB052}" name="peer_cidrs" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{A49490F8-FF19-4247-A9DC-3E9A8C9508D2}" name="admin_state_up" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{D393C6C1-4F72-964B-9D76-BE2A1539821D}" name="dead_peer_action" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{D523FCFB-A055-084E-B6ED-C788AB1D158E}" name="dead_peer_interval" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{9A0739C3-7687-E94A-984F-5C145DFE3E89}" name="dead_peer_timeout" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{ACD56801-B98E-7847-85C3-F2FFBA76F061}" name="ike_policy" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{1BD10945-B68C-DF4E-AA5E-ACEC66F06E3C}" name="ipsec_policy" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{4B0694AF-1BD1-694F-90B1-B1A9567550B0}" name="delete_timeout" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{C4B8842B-2BB7-EB49-B6D2-B6721C54DC5F}" name="*name" dataDxfId="33"/>
+    <tableColumn id="13" xr3:uid="{78EC6C87-C780-E34D-BBD5-54ED244AB6D6}" name="*vpn_gateway" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{DBBB9AC2-20E7-974C-935D-20C40D819A02}" name="*peer_address" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{5CDA888D-9763-CE46-98E3-D4B85974B5A5}" name="*preshared_key" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{D1C2C80B-E944-E049-AD39-98867623465E}" name="local_cidrs" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{B6F5AA94-6774-DA4F-8D22-7820C9CFB052}" name="peer_cidrs" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{A49490F8-FF19-4247-A9DC-3E9A8C9508D2}" name="admin_state_up" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{D393C6C1-4F72-964B-9D76-BE2A1539821D}" name="dead_peer_action" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{D523FCFB-A055-084E-B6ED-C788AB1D158E}" name="dead_peer_interval" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{9A0739C3-7687-E94A-984F-5C145DFE3E89}" name="dead_peer_timeout" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{ACD56801-B98E-7847-85C3-F2FFBA76F061}" name="ike_policy" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{1BD10945-B68C-DF4E-AA5E-ACEC66F06E3C}" name="ipsec_policy" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{4B0694AF-1BD1-694F-90B1-B1A9567550B0}" name="delete_timeout" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4C9E897C-45DC-AA46-A7F0-E0156EB5EE87}" name="Table4" displayName="Table4" ref="A1:F2" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:F2" xr:uid="{CCD253BB-BDC0-6D49-A9E2-C5B81CFC6DEA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{48612795-253E-2045-9A1C-B75C9BF5816E}" name="Table111" displayName="Table111" ref="A1:F3" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:F3" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E78C0226-94B1-2F4F-B660-7B46E3C209D7}" name="*name" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{853CCA70-7549-8348-B2F0-E0B9673C117C}" name="*authentication_algorithm" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{7C537180-3AF2-7D49-B452-4B95360755FA}" name="*encryption_algorithm" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{57683AF3-88F5-1742-A5BC-A9D2829B75AF}" name="*pfs" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{0C3F595F-188C-3F44-A3A6-18FFE3328F8E}" name="key_lifetime" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{E4657436-73F2-644C-868F-F09AE522C958}" name="resource_group" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{73198180-EC4B-3448-8FD7-AD7FE682C21E}" name="*name" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{A3F85132-9C0A-074A-AD1C-FC8C58C48C9A}" name="*authentication_algorithm" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{E34718FD-92F0-1A43-80D5-70140F486148}" name="*encryption_algorithm" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{42FD0836-3534-9647-8D8D-7A54E0E1C7AA}" name="*pfs" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{59778D38-F5AC-AC4E-845F-BC7470387817}" name="key_lifetime" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{BABC3429-E57A-4F47-92E7-58CB470AF7F9}" name="resource_group" dataDxfId="9"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{7CBBDF02-B318-9E4C-BB23-512C9854A463}" name="Table5" displayName="Table5" ref="A1:G2" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G2" xr:uid="{3C25B185-B5C0-214E-B804-802BB0A8BEDD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EE4FC002-D07C-9447-9703-8452CE1C018E}" name="Table11112" displayName="Table11112" ref="A1:G3" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G3" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{89E95447-F298-4C47-87E5-4FC55EF0AF7A}" name="*name" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{0EA20FB6-25F7-284E-8CC5-4CB401EDE97A}" name="*authentication_algorithm" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{65E99A3C-D50C-1D4A-92C4-1E9025F0817D}" name="*encryption_algorithm" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{8F898F33-8CA1-B341-9DDF-EFB3DB73D836}" name="*dh_group" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{3BC498C0-C926-304C-8FFE-BF895CB946E6}" name="ike_version" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{0AB50BA7-934F-694C-BCAA-521093AFBAC2}" name="key_lifetime" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{A97197C9-1F7F-B841-B830-11A35CF47F35}" name="resource_group" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{06812B35-A623-5241-A8DF-8EEB6166846D}" name="*name" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{9551CB52-166F-6E47-9A17-EC3E828FEB2C}" name="*authentication_algorithm" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{246BA229-88CD-0A4B-AD52-5F86AA06873E}" name="*encryption_algorithm" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{2E993777-DA48-4C4D-B929-49BFFB90F9D0}" name="*dh_group" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{A6127979-DB02-954A-BE3A-277928AF4686}" name="ike_version" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{1E691E85-EB8B-A64D-B4A6-22E7A68094F6}" name="key_lifetime" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{9B4820A8-622D-1540-A53E-6FCBAB87C546}" name="resource_group" dataDxfId="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0501486B-99D9-D847-9265-3A1B8C4F9CB7}" name="Table32" displayName="Table32" ref="A1:B2" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
-  <autoFilter ref="A1:B2" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0501486B-99D9-D847-9265-3A1B8C4F9CB7}" name="Table32" displayName="Table32" ref="A1:B3" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:B3" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2B5EBF30-5208-5D4D-BE48-42C200D7DA49}" name="*name" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{593C94B9-EB1B-0945-A6EA-29933D3679F2}" name="tags" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{2B5EBF30-5208-5D4D-BE48-42C200D7DA49}" name="*name" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{593C94B9-EB1B-0945-A6EA-29933D3679F2}" name="tags" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1312,7 +1310,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682C37B2-7460-6E41-82EB-016F50EC9459}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1337,6 +1335,10 @@
         <v>33</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1347,7 +1349,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00818959-CEA4-3842-8CDF-BB71D693A9FD}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1393,6 +1395,11 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1403,14 +1410,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97FDD6D-C176-5945-B0CF-4B4E2F084837}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="7" max="9" width="20.83203125" customWidth="1"/>
+    <col min="7" max="10" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -1513,6 +1520,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
@@ -1528,6 +1536,20 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1537,22 +1559,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E18E747-91FB-8F41-89A5-1E5E6B386BA6}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E931148C-7425-8142-A16D-7BBA174CE38C}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1569,10 +1591,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1585,6 +1607,14 @@
         <v>3600</v>
       </c>
       <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1595,22 +1625,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B7C484-5612-D44A-82D4-955EC5E05A32}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C836A2-0C93-8B42-8C00-3FFAF090CB9E}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1630,10 +1660,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1649,6 +1679,15 @@
         <v>28800</v>
       </c>
       <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1660,7 +1699,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D793E16-396D-2241-B738-EC8BCCA2DB01}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1681,6 +1720,10 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
updated mac version to 1.2.0.0
</commit_message>
<xml_diff>
--- a/examples/access.xlsx
+++ b/examples/access.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1848DA-0A1C-A447-B525-F03AEE946E10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0383CF-4308-F548-8750-8ECC7CB06A4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7700" yWindow="460" windowWidth="25600" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="4900" windowWidth="25600" windowHeight="14700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="aclrules" sheetId="51" r:id="rId1"/>
-    <sheet name="sgheaders" sheetId="53" r:id="rId2"/>
-    <sheet name="sgrules" sheetId="52" r:id="rId3"/>
-    <sheet name="sshkeys" sheetId="55" r:id="rId4"/>
-    <sheet name="vpngateways" sheetId="56" r:id="rId5"/>
-    <sheet name="vpnconnections" sheetId="57" r:id="rId6"/>
-    <sheet name="ipsecpolicies" sheetId="60" r:id="rId7"/>
-    <sheet name="ikepolicies" sheetId="61" r:id="rId8"/>
-    <sheet name="resourcegroups" sheetId="54" r:id="rId9"/>
+    <sheet name="aclheaders" sheetId="62" r:id="rId1"/>
+    <sheet name="aclrules" sheetId="51" r:id="rId2"/>
+    <sheet name="sgheaders" sheetId="53" r:id="rId3"/>
+    <sheet name="sgrules" sheetId="52" r:id="rId4"/>
+    <sheet name="sshkeys" sheetId="55" r:id="rId5"/>
+    <sheet name="vpngateways" sheetId="56" r:id="rId6"/>
+    <sheet name="vpnconnections" sheetId="57" r:id="rId7"/>
+    <sheet name="ipsecpolicies" sheetId="60" r:id="rId8"/>
+    <sheet name="ikepolicies" sheetId="61" r:id="rId9"/>
+    <sheet name="resourcegroups" sheetId="54" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
   <si>
     <t>*name</t>
   </si>
@@ -307,22 +308,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="72">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -339,6 +325,10 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -379,13 +369,24 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -501,6 +502,9 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -622,6 +626,39 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -636,60 +673,83 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8524F582-25D9-D64B-A9C7-4FF4A27248B3}" name="Table1" displayName="Table1" ref="A1:G4" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
-  <autoFilter ref="A1:G4" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{36FEA897-58B8-8244-BBD2-F934FDEC8E9A}" name="*name" dataDxfId="64"/>
-    <tableColumn id="6" xr3:uid="{C499C2EF-3238-4B4A-8017-492B9A1A77FF}" name="*acl" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{F12A4B82-233E-A440-B918-86C5E4C82FD9}" name="*action" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{568185F1-B557-2C49-B724-A15618F6D5DE}" name="*source" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{F5A78E34-0750-6E4E-BE76-F9B327F65E12}" name="*destination" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{83261B25-C691-8D45-8989-863A46F2510F}" name="*direction" dataDxfId="59"/>
-    <tableColumn id="11" xr3:uid="{DA919A14-BC6E-5547-A993-1B7855521094}" name="protocol" dataDxfId="58"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{C01606B7-BCCF-0641-95B9-33736AB784F9}" name="Table1849" displayName="Table1849" ref="A1:B2" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+  <autoFilter ref="A1:B2" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{039F5A72-2E04-E045-9C9A-D435D378174B}" name="*name" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{7818DB98-2599-904B-BA0F-0790B6E1B3E4}" name="*vpc" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83144CBC-65AD-804B-B36C-148A65E84D16}" name="Table184" displayName="Table184" ref="A1:C3" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
-  <autoFilter ref="A1:C3" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A724ADCC-F039-0D45-9937-58B50BC5715E}" name="*name" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{B9D7A6DC-911D-B749-AE7A-2DC2D907D356}" name="*vpc" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{CE9B4557-50B5-2A4A-AA03-F9F781F4F349}" name="resource_group" dataDxfId="53"/>
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0501486B-99D9-D847-9265-3A1B8C4F9CB7}" name="Table32" displayName="Table32" ref="A1:B3" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A1:B3" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{2B5EBF30-5208-5D4D-BE48-42C200D7DA49}" name="*name" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{593C94B9-EB1B-0945-A6EA-29933D3679F2}" name="tags" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11008CC8-5C85-3B48-82BD-CD830AD3D6DF}" name="Table18" displayName="Table18" ref="A1:F6" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
-  <autoFilter ref="A1:F6" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{203C77A6-285B-124C-AF24-A3511F6244F7}" name="*name" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{2F8C3C4B-0E49-4A4D-AC20-F814AA26DD74}" name="*group" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{42DAC7A2-384A-144A-9BDC-F241D22F7F74}" name="*direction" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{41DCA0FA-BF94-6343-BF46-01D165299C09}" name="*remote" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{15B7721A-4EE3-9847-9C27-38416048A9AE}" name="ip_version" dataDxfId="46"/>
-    <tableColumn id="10" xr3:uid="{F2B3B9EB-B923-1342-8152-241A84E63D18}" name="protocol" dataDxfId="45"/>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8524F582-25D9-D64B-A9C7-4FF4A27248B3}" name="Table1" displayName="Table1" ref="A1:G4" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+  <autoFilter ref="A1:G4" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{36FEA897-58B8-8244-BBD2-F934FDEC8E9A}" name="*name" dataDxfId="65"/>
+    <tableColumn id="6" xr3:uid="{C499C2EF-3238-4B4A-8017-492B9A1A77FF}" name="*acl" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{F12A4B82-233E-A440-B918-86C5E4C82FD9}" name="*action" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{568185F1-B557-2C49-B724-A15618F6D5DE}" name="*source" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{F5A78E34-0750-6E4E-BE76-F9B327F65E12}" name="*destination" dataDxfId="61"/>
+    <tableColumn id="5" xr3:uid="{83261B25-C691-8D45-8989-863A46F2510F}" name="*direction" dataDxfId="60"/>
+    <tableColumn id="11" xr3:uid="{DA919A14-BC6E-5547-A993-1B7855521094}" name="protocol" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D0CA34BD-A489-B54D-8D4B-B907D54F9FC9}" name="Table3" displayName="Table3" ref="A1:B3" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
-  <autoFilter ref="A1:B3" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FC67A5D3-A34E-3D4E-9E86-D02090ED17CB}" name="*name" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{F56C754B-0F5D-694F-BD5D-7925CDFC5F97}" name="*public_key" dataDxfId="41"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83144CBC-65AD-804B-B36C-148A65E84D16}" name="Table184" displayName="Table184" ref="A1:C3" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+  <autoFilter ref="A1:C3" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A724ADCC-F039-0D45-9937-58B50BC5715E}" name="*name" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{B9D7A6DC-911D-B749-AE7A-2DC2D907D356}" name="*vpc" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{CE9B4557-50B5-2A4A-AA03-F9F781F4F349}" name="resource_group" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11008CC8-5C85-3B48-82BD-CD830AD3D6DF}" name="Table18" displayName="Table18" ref="A1:F6" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+  <autoFilter ref="A1:F6" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{203C77A6-285B-124C-AF24-A3511F6244F7}" name="*name" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{2F8C3C4B-0E49-4A4D-AC20-F814AA26DD74}" name="*group" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{42DAC7A2-384A-144A-9BDC-F241D22F7F74}" name="*direction" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{41DCA0FA-BF94-6343-BF46-01D165299C09}" name="*remote" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{15B7721A-4EE3-9847-9C27-38416048A9AE}" name="ip_version" dataDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{F2B3B9EB-B923-1342-8152-241A84E63D18}" name="protocol" dataDxfId="46"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D0CA34BD-A489-B54D-8D4B-B907D54F9FC9}" name="Table3" displayName="Table3" ref="A1:C3" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+  <autoFilter ref="A1:C3" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{FC67A5D3-A34E-3D4E-9E86-D02090ED17CB}" name="*name" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{F56C754B-0F5D-694F-BD5D-7925CDFC5F97}" name="*public_key" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{FDE02962-4673-2D4C-AFB9-1D7FCFCC6AA0}" name="resource_group" dataDxfId="41"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{74F9BE67-E011-B34A-A492-0717499F0410}" name="Table16" displayName="Table16" ref="A1:C3" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="A1:C3" xr:uid="{6D379596-E186-C240-BBB4-B8E74F1D3D56}"/>
   <tableColumns count="3">
@@ -701,7 +761,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B4318CDD-C98E-1341-88CD-5334A857D418}" name="Table15" displayName="Table15" ref="A1:M3" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A1:M3" xr:uid="{27D8B65D-C3AF-BD4B-8BB7-5754C974B57F}"/>
   <tableColumns count="13">
@@ -723,43 +783,32 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{48612795-253E-2045-9A1C-B75C9BF5816E}" name="Table111" displayName="Table111" ref="A1:F3" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{48612795-253E-2045-9A1C-B75C9BF5816E}" name="Table111" displayName="Table111" ref="A1:F3" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:F3" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{73198180-EC4B-3448-8FD7-AD7FE682C21E}" name="*name" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{A3F85132-9C0A-074A-AD1C-FC8C58C48C9A}" name="*authentication_algorithm" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{E34718FD-92F0-1A43-80D5-70140F486148}" name="*encryption_algorithm" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{42FD0836-3534-9647-8D8D-7A54E0E1C7AA}" name="*pfs" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{59778D38-F5AC-AC4E-845F-BC7470387817}" name="key_lifetime" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{BABC3429-E57A-4F47-92E7-58CB470AF7F9}" name="resource_group" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{73198180-EC4B-3448-8FD7-AD7FE682C21E}" name="*name" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{A3F85132-9C0A-074A-AD1C-FC8C58C48C9A}" name="*authentication_algorithm" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{E34718FD-92F0-1A43-80D5-70140F486148}" name="*encryption_algorithm" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{42FD0836-3534-9647-8D8D-7A54E0E1C7AA}" name="*pfs" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{59778D38-F5AC-AC4E-845F-BC7470387817}" name="key_lifetime" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{BABC3429-E57A-4F47-92E7-58CB470AF7F9}" name="resource_group" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EE4FC002-D07C-9447-9703-8452CE1C018E}" name="Table11112" displayName="Table11112" ref="A1:G3" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EE4FC002-D07C-9447-9703-8452CE1C018E}" name="Table11112" displayName="Table11112" ref="A1:G3" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:G3" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{06812B35-A623-5241-A8DF-8EEB6166846D}" name="*name" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{9551CB52-166F-6E47-9A17-EC3E828FEB2C}" name="*authentication_algorithm" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{246BA229-88CD-0A4B-AD52-5F86AA06873E}" name="*encryption_algorithm" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{2E993777-DA48-4C4D-B929-49BFFB90F9D0}" name="*dh_group" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{A6127979-DB02-954A-BE3A-277928AF4686}" name="ike_version" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{1E691E85-EB8B-A64D-B4A6-22E7A68094F6}" name="key_lifetime" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{9B4820A8-622D-1540-A53E-6FCBAB87C546}" name="resource_group" dataDxfId="2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0501486B-99D9-D847-9265-3A1B8C4F9CB7}" name="Table32" displayName="Table32" ref="A1:B3" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:B3" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2B5EBF30-5208-5D4D-BE48-42C200D7DA49}" name="*name" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{593C94B9-EB1B-0945-A6EA-29933D3679F2}" name="tags" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{06812B35-A623-5241-A8DF-8EEB6166846D}" name="*name" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{9551CB52-166F-6E47-9A17-EC3E828FEB2C}" name="*authentication_algorithm" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{246BA229-88CD-0A4B-AD52-5F86AA06873E}" name="*encryption_algorithm" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{2E993777-DA48-4C4D-B929-49BFFB90F9D0}" name="*dh_group" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{A6127979-DB02-954A-BE3A-277928AF4686}" name="ike_version" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{1E691E85-EB8B-A64D-B4A6-22E7A68094F6}" name="key_lifetime" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{9B4820A8-622D-1540-A53E-6FCBAB87C546}" name="resource_group" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1027,6 +1076,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515B7804-FA89-F84C-8321-3F26CCBED84F}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D793E16-396D-2241-B738-EC8BCCA2DB01}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB3C17B-7688-8D45-9DEE-F9650DD6901F}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1076,9 +1202,7 @@
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -1099,9 +1223,7 @@
       <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1132,7 +1254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F29E99F-EAC6-EF42-BBDE-1489EAD1BB17}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1185,7 +1307,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3D3370-44D8-0A42-8C42-E9D4E75B0DB2}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -1308,9 +1430,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682C37B2-7460-6E41-82EB-016F50EC9459}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1319,25 +1441,30 @@
     <col min="2" max="2" width="33.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1347,7 +1474,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00818959-CEA4-3842-8CDF-BB71D693A9FD}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -1408,11 +1535,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97FDD6D-C176-5945-B0CF-4B4E2F084837}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="H1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1558,7 +1685,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E931148C-7425-8142-A16D-7BBA174CE38C}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1624,7 +1751,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C836A2-0C93-8B42-8C00-3FFAF090CB9E}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1695,39 +1822,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D793E16-396D-2241-B738-EC8BCCA2DB01}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated mac version to 1.2.0.1
</commit_message>
<xml_diff>
--- a/examples/access.xlsx
+++ b/examples/access.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0383CF-4308-F548-8750-8ECC7CB06A4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAD5026-F717-A443-82C9-2D0DCBF16940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="4900" windowWidth="25600" windowHeight="14700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="-17560" windowWidth="25600" windowHeight="14700" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aclheaders" sheetId="62" r:id="rId1"/>
@@ -673,8 +673,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{C01606B7-BCCF-0641-95B9-33736AB784F9}" name="Table1849" displayName="Table1849" ref="A1:B2" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
-  <autoFilter ref="A1:B2" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{C01606B7-BCCF-0641-95B9-33736AB784F9}" name="Table1849" displayName="Table1849" ref="A1:B3" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+  <autoFilter ref="A1:B3" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{039F5A72-2E04-E045-9C9A-D435D378174B}" name="*name" dataDxfId="69"/>
     <tableColumn id="2" xr3:uid="{7818DB98-2599-904B-BA0F-0790B6E1B3E4}" name="*vpc" dataDxfId="68"/>
@@ -1077,7 +1077,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515B7804-FA89-F84C-8321-3F26CCBED84F}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1104,9 +1104,15 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1121,7 +1127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D793E16-396D-2241-B738-EC8BCCA2DB01}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1156,7 +1162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB3C17B-7688-8D45-9DEE-F9650DD6901F}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
updated mac version to 1.2.1.0
</commit_message>
<xml_diff>
--- a/examples/access.xlsx
+++ b/examples/access.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAD5026-F717-A443-82C9-2D0DCBF16940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C45FFB1-671E-834D-93A3-8A7B5C4B7358}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="-17560" windowWidth="25600" windowHeight="14700" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8080" yWindow="560" windowWidth="25600" windowHeight="14820" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aclheaders" sheetId="62" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="70">
   <si>
     <t>*name</t>
   </si>
@@ -63,12 +63,6 @@
     <t>inbound</t>
   </si>
   <si>
-    <t>tcp:80:80</t>
-  </si>
-  <si>
-    <t>udp:805:807</t>
-  </si>
-  <si>
     <t>outbound</t>
   </si>
   <si>
@@ -226,13 +220,37 @@
   </si>
   <si>
     <t>ikepolicy1</t>
+  </si>
+  <si>
+    <t>icmp_code</t>
+  </si>
+  <si>
+    <t>icmp_type</t>
+  </si>
+  <si>
+    <t>port_min</t>
+  </si>
+  <si>
+    <t>port_max</t>
+  </si>
+  <si>
+    <t>source_port_min</t>
+  </si>
+  <si>
+    <t>source_port_max</t>
+  </si>
+  <si>
+    <t>tcp</t>
+  </si>
+  <si>
+    <t>udp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +261,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -308,7 +332,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="72">
+  <dxfs count="85">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -535,6 +562,24 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -619,6 +664,24 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -673,142 +736,155 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{C01606B7-BCCF-0641-95B9-33736AB784F9}" name="Table1849" displayName="Table1849" ref="A1:B3" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{C01606B7-BCCF-0641-95B9-33736AB784F9}" name="Table1849" displayName="Table1849" ref="A1:B3" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83">
   <autoFilter ref="A1:B3" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{039F5A72-2E04-E045-9C9A-D435D378174B}" name="*name" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{7818DB98-2599-904B-BA0F-0790B6E1B3E4}" name="*vpc" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{039F5A72-2E04-E045-9C9A-D435D378174B}" name="*name" dataDxfId="82"/>
+    <tableColumn id="2" xr3:uid="{7818DB98-2599-904B-BA0F-0790B6E1B3E4}" name="*vpc" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0501486B-99D9-D847-9265-3A1B8C4F9CB7}" name="Table32" displayName="Table32" ref="A1:B3" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0501486B-99D9-D847-9265-3A1B8C4F9CB7}" name="Table32" displayName="Table32" ref="A1:B3" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:B3" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2B5EBF30-5208-5D4D-BE48-42C200D7DA49}" name="*name" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{593C94B9-EB1B-0945-A6EA-29933D3679F2}" name="tags" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{2B5EBF30-5208-5D4D-BE48-42C200D7DA49}" name="*name" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{593C94B9-EB1B-0945-A6EA-29933D3679F2}" name="tags" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8524F582-25D9-D64B-A9C7-4FF4A27248B3}" name="Table1" displayName="Table1" ref="A1:G4" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
-  <autoFilter ref="A1:G4" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{36FEA897-58B8-8244-BBD2-F934FDEC8E9A}" name="*name" dataDxfId="65"/>
-    <tableColumn id="6" xr3:uid="{C499C2EF-3238-4B4A-8017-492B9A1A77FF}" name="*acl" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{F12A4B82-233E-A440-B918-86C5E4C82FD9}" name="*action" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{568185F1-B557-2C49-B724-A15618F6D5DE}" name="*source" dataDxfId="62"/>
-    <tableColumn id="4" xr3:uid="{F5A78E34-0750-6E4E-BE76-F9B327F65E12}" name="*destination" dataDxfId="61"/>
-    <tableColumn id="5" xr3:uid="{83261B25-C691-8D45-8989-863A46F2510F}" name="*direction" dataDxfId="60"/>
-    <tableColumn id="11" xr3:uid="{DA919A14-BC6E-5547-A993-1B7855521094}" name="protocol" dataDxfId="59"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8524F582-25D9-D64B-A9C7-4FF4A27248B3}" name="Table1" displayName="Table1" ref="A1:M4" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
+  <autoFilter ref="A1:M4" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{36FEA897-58B8-8244-BBD2-F934FDEC8E9A}" name="*name" dataDxfId="78"/>
+    <tableColumn id="6" xr3:uid="{C499C2EF-3238-4B4A-8017-492B9A1A77FF}" name="*acl" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{F12A4B82-233E-A440-B918-86C5E4C82FD9}" name="*action" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{568185F1-B557-2C49-B724-A15618F6D5DE}" name="*source" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{F5A78E34-0750-6E4E-BE76-F9B327F65E12}" name="*destination" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{83261B25-C691-8D45-8989-863A46F2510F}" name="*direction" dataDxfId="73"/>
+    <tableColumn id="14" xr3:uid="{BF39CD2E-14E9-4A43-A8D3-BBB3BB29D4E4}" name="protocol" dataDxfId="72"/>
+    <tableColumn id="10" xr3:uid="{5AAB00B2-E1E7-9E40-98F1-D7B64B119564}" name="port_min" dataDxfId="71"/>
+    <tableColumn id="9" xr3:uid="{61B251A9-3DF1-3543-868E-D48BC0D2FBE8}" name="port_max" dataDxfId="70"/>
+    <tableColumn id="12" xr3:uid="{DA76B0C3-0D2A-2C42-A980-F1A40B9E72F2}" name="source_port_min" dataDxfId="69"/>
+    <tableColumn id="11" xr3:uid="{DA919A14-BC6E-5547-A993-1B7855521094}" name="source_port_max" dataDxfId="68"/>
+    <tableColumn id="13" xr3:uid="{902C025B-6D2D-EA4A-B172-E87E77CC4CDC}" name="icmp_code" dataDxfId="67"/>
+    <tableColumn id="15" xr3:uid="{E1C798F8-B37C-A14A-A32A-18E35BCC086A}" name="icmp_type" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83144CBC-65AD-804B-B36C-148A65E84D16}" name="Table184" displayName="Table184" ref="A1:C3" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83144CBC-65AD-804B-B36C-148A65E84D16}" name="Table184" displayName="Table184" ref="A1:C3" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
   <autoFilter ref="A1:C3" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A724ADCC-F039-0D45-9937-58B50BC5715E}" name="*name" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{B9D7A6DC-911D-B749-AE7A-2DC2D907D356}" name="*vpc" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{CE9B4557-50B5-2A4A-AA03-F9F781F4F349}" name="resource_group" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{A724ADCC-F039-0D45-9937-58B50BC5715E}" name="*name" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{B9D7A6DC-911D-B749-AE7A-2DC2D907D356}" name="*vpc" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{CE9B4557-50B5-2A4A-AA03-F9F781F4F349}" name="resource_group" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11008CC8-5C85-3B48-82BD-CD830AD3D6DF}" name="Table18" displayName="Table18" ref="A1:F6" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
-  <autoFilter ref="A1:F6" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{203C77A6-285B-124C-AF24-A3511F6244F7}" name="*name" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{2F8C3C4B-0E49-4A4D-AC20-F814AA26DD74}" name="*group" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{42DAC7A2-384A-144A-9BDC-F241D22F7F74}" name="*direction" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{41DCA0FA-BF94-6343-BF46-01D165299C09}" name="*remote" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{15B7721A-4EE3-9847-9C27-38416048A9AE}" name="ip_version" dataDxfId="47"/>
-    <tableColumn id="10" xr3:uid="{F2B3B9EB-B923-1342-8152-241A84E63D18}" name="protocol" dataDxfId="46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11008CC8-5C85-3B48-82BD-CD830AD3D6DF}" name="Table18" displayName="Table18" ref="A1:L6" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+  <autoFilter ref="A1:L6" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{203C77A6-285B-124C-AF24-A3511F6244F7}" name="*name" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{2F8C3C4B-0E49-4A4D-AC20-F814AA26DD74}" name="*group" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{42DAC7A2-384A-144A-9BDC-F241D22F7F74}" name="*direction" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{41DCA0FA-BF94-6343-BF46-01D165299C09}" name="*remote" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{15B7721A-4EE3-9847-9C27-38416048A9AE}" name="ip_version" dataDxfId="54"/>
+    <tableColumn id="11" xr3:uid="{FE5D1059-98EB-6246-BC1E-22FD29D3D313}" name="protocol" dataDxfId="53"/>
+    <tableColumn id="7" xr3:uid="{DEE8533C-7DBB-6B4E-95DA-ADF92BBA34C8}" name="port_min" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{9B67B5CE-A552-3B4B-A870-AA27F074FBE8}" name="port_max" dataDxfId="51"/>
+    <tableColumn id="13" xr3:uid="{6622CF72-D1A7-4B42-80B1-9F946BD4E07F}" name="source_port_min" dataDxfId="50"/>
+    <tableColumn id="12" xr3:uid="{3842F58E-9ADA-E74C-8636-BB12452EBA78}" name="source_port_max" dataDxfId="49"/>
+    <tableColumn id="10" xr3:uid="{4B9F59F6-DF24-EC4C-8C45-5F37270DACD5}" name="icmp_code" dataDxfId="48"/>
+    <tableColumn id="14" xr3:uid="{9D813CAB-D3ED-D84E-98F7-81A78541F29B}" name="icmp_type" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D0CA34BD-A489-B54D-8D4B-B907D54F9FC9}" name="Table3" displayName="Table3" ref="A1:C3" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
-  <autoFilter ref="A1:C3" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FC67A5D3-A34E-3D4E-9E86-D02090ED17CB}" name="*name" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{F56C754B-0F5D-694F-BD5D-7925CDFC5F97}" name="*public_key" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{FDE02962-4673-2D4C-AFB9-1D7FCFCC6AA0}" name="resource_group" dataDxfId="41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D0CA34BD-A489-B54D-8D4B-B907D54F9FC9}" name="Table3" displayName="Table3" ref="A1:D3" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+  <autoFilter ref="A1:D3" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{FC67A5D3-A34E-3D4E-9E86-D02090ED17CB}" name="*name" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{F56C754B-0F5D-694F-BD5D-7925CDFC5F97}" name="*public_key" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{FDE02962-4673-2D4C-AFB9-1D7FCFCC6AA0}" name="resource_group" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{79F1DE46-3AC5-284E-8E48-AA0D55380DFD}" name="tags" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{74F9BE67-E011-B34A-A492-0717499F0410}" name="Table16" displayName="Table16" ref="A1:C3" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{74F9BE67-E011-B34A-A492-0717499F0410}" name="Table16" displayName="Table16" ref="A1:C3" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A1:C3" xr:uid="{6D379596-E186-C240-BBB4-B8E74F1D3D56}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{5FD29999-A9F5-C549-98A3-DFD2B1437449}" name="*name" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{35CF1270-9B78-4243-98F7-E702702F38FF}" name="*subnet" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{B806F889-718F-584A-ADDF-8A3AD802CDFB}" name="resource_group" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{5FD29999-A9F5-C549-98A3-DFD2B1437449}" name="*name" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{35CF1270-9B78-4243-98F7-E702702F38FF}" name="*subnet" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{B806F889-718F-584A-ADDF-8A3AD802CDFB}" name="resource_group" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B4318CDD-C98E-1341-88CD-5334A857D418}" name="Table15" displayName="Table15" ref="A1:M3" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B4318CDD-C98E-1341-88CD-5334A857D418}" name="Table15" displayName="Table15" ref="A1:M3" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="A1:M3" xr:uid="{27D8B65D-C3AF-BD4B-8BB7-5754C974B57F}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{C4B8842B-2BB7-EB49-B6D2-B6721C54DC5F}" name="*name" dataDxfId="33"/>
-    <tableColumn id="13" xr3:uid="{78EC6C87-C780-E34D-BBD5-54ED244AB6D6}" name="*vpn_gateway" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{DBBB9AC2-20E7-974C-935D-20C40D819A02}" name="*peer_address" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{5CDA888D-9763-CE46-98E3-D4B85974B5A5}" name="*preshared_key" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{D1C2C80B-E944-E049-AD39-98867623465E}" name="local_cidrs" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{B6F5AA94-6774-DA4F-8D22-7820C9CFB052}" name="peer_cidrs" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{A49490F8-FF19-4247-A9DC-3E9A8C9508D2}" name="admin_state_up" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{D393C6C1-4F72-964B-9D76-BE2A1539821D}" name="dead_peer_action" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{D523FCFB-A055-084E-B6ED-C788AB1D158E}" name="dead_peer_interval" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{9A0739C3-7687-E94A-984F-5C145DFE3E89}" name="dead_peer_timeout" dataDxfId="24"/>
-    <tableColumn id="10" xr3:uid="{ACD56801-B98E-7847-85C3-F2FFBA76F061}" name="ike_policy" dataDxfId="23"/>
-    <tableColumn id="11" xr3:uid="{1BD10945-B68C-DF4E-AA5E-ACEC66F06E3C}" name="ipsec_policy" dataDxfId="22"/>
-    <tableColumn id="12" xr3:uid="{4B0694AF-1BD1-694F-90B1-B1A9567550B0}" name="delete_timeout" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{C4B8842B-2BB7-EB49-B6D2-B6721C54DC5F}" name="*name" dataDxfId="34"/>
+    <tableColumn id="13" xr3:uid="{78EC6C87-C780-E34D-BBD5-54ED244AB6D6}" name="*vpn_gateway" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{DBBB9AC2-20E7-974C-935D-20C40D819A02}" name="*peer_address" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{5CDA888D-9763-CE46-98E3-D4B85974B5A5}" name="*preshared_key" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{D1C2C80B-E944-E049-AD39-98867623465E}" name="local_cidrs" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{B6F5AA94-6774-DA4F-8D22-7820C9CFB052}" name="peer_cidrs" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{A49490F8-FF19-4247-A9DC-3E9A8C9508D2}" name="admin_state_up" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{D393C6C1-4F72-964B-9D76-BE2A1539821D}" name="dead_peer_action" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{D523FCFB-A055-084E-B6ED-C788AB1D158E}" name="dead_peer_interval" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{9A0739C3-7687-E94A-984F-5C145DFE3E89}" name="dead_peer_timeout" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{ACD56801-B98E-7847-85C3-F2FFBA76F061}" name="ike_policy" dataDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{1BD10945-B68C-DF4E-AA5E-ACEC66F06E3C}" name="ipsec_policy" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{4B0694AF-1BD1-694F-90B1-B1A9567550B0}" name="delete_timeout" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{48612795-253E-2045-9A1C-B75C9BF5816E}" name="Table111" displayName="Table111" ref="A1:F3" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{48612795-253E-2045-9A1C-B75C9BF5816E}" name="Table111" displayName="Table111" ref="A1:F3" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:F3" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{73198180-EC4B-3448-8FD7-AD7FE682C21E}" name="*name" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{A3F85132-9C0A-074A-AD1C-FC8C58C48C9A}" name="*authentication_algorithm" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{E34718FD-92F0-1A43-80D5-70140F486148}" name="*encryption_algorithm" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{42FD0836-3534-9647-8D8D-7A54E0E1C7AA}" name="*pfs" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{59778D38-F5AC-AC4E-845F-BC7470387817}" name="key_lifetime" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{BABC3429-E57A-4F47-92E7-58CB470AF7F9}" name="resource_group" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{73198180-EC4B-3448-8FD7-AD7FE682C21E}" name="*name" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{A3F85132-9C0A-074A-AD1C-FC8C58C48C9A}" name="*authentication_algorithm" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{E34718FD-92F0-1A43-80D5-70140F486148}" name="*encryption_algorithm" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{42FD0836-3534-9647-8D8D-7A54E0E1C7AA}" name="*pfs" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{59778D38-F5AC-AC4E-845F-BC7470387817}" name="key_lifetime" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{BABC3429-E57A-4F47-92E7-58CB470AF7F9}" name="resource_group" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EE4FC002-D07C-9447-9703-8452CE1C018E}" name="Table11112" displayName="Table11112" ref="A1:G3" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EE4FC002-D07C-9447-9703-8452CE1C018E}" name="Table11112" displayName="Table11112" ref="A1:G3" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:G3" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{06812B35-A623-5241-A8DF-8EEB6166846D}" name="*name" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{9551CB52-166F-6E47-9A17-EC3E828FEB2C}" name="*authentication_algorithm" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{246BA229-88CD-0A4B-AD52-5F86AA06873E}" name="*encryption_algorithm" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{2E993777-DA48-4C4D-B929-49BFFB90F9D0}" name="*dh_group" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{A6127979-DB02-954A-BE3A-277928AF4686}" name="ike_version" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{1E691E85-EB8B-A64D-B4A6-22E7A68094F6}" name="key_lifetime" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{9B4820A8-622D-1540-A53E-6FCBAB87C546}" name="resource_group" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{06812B35-A623-5241-A8DF-8EEB6166846D}" name="*name" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{9551CB52-166F-6E47-9A17-EC3E828FEB2C}" name="*authentication_algorithm" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{246BA229-88CD-0A4B-AD52-5F86AA06873E}" name="*encryption_algorithm" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{2E993777-DA48-4C4D-B929-49BFFB90F9D0}" name="*dh_group" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{A6127979-DB02-954A-BE3A-277928AF4686}" name="ike_version" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{1E691E85-EB8B-A64D-B4A6-22E7A68094F6}" name="key_lifetime" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{9B4820A8-622D-1540-A53E-6FCBAB87C546}" name="resource_group" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1088,15 +1164,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1127,7 +1203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D793E16-396D-2241-B738-EC8BCCA2DB01}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1139,7 +1215,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1160,18 +1236,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB3C17B-7688-8D45-9DEE-F9650DD6901F}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="9" width="12.83203125" customWidth="1"/>
+    <col min="10" max="11" width="16.83203125" customWidth="1"/>
+    <col min="12" max="13" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1188,13 +1269,31 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -1208,14 +1307,26 @@
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="1">
+        <v>80</v>
+      </c>
+      <c r="I2" s="1">
+        <v>80</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -1229,14 +1340,26 @@
       <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="1">
+        <v>805</v>
+      </c>
+      <c r="I3" s="1">
+        <v>807</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -1248,11 +1371,18 @@
         <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1273,27 +1403,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1315,112 +1445,171 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3D3370-44D8-0A42-8C42-E9D4E75B0DB2}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="10" width="16.83203125" customWidth="1"/>
+    <col min="11" max="14" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="1">
+        <v>80</v>
+      </c>
+      <c r="H2" s="1">
+        <v>80</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="G3" s="1">
+        <v>805</v>
+      </c>
+      <c r="H3" s="1">
+        <v>807</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1428,6 +1617,7 @@
       <c r="E7" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -1438,39 +1628,44 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682C37B2-7460-6E41-82EB-016F50EC9459}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="33.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1499,18 +1694,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1558,60 +1753,60 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1619,10 +1814,10 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1708,33 +1903,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="E2" s="1">
         <v>3600</v>
@@ -1774,33 +1969,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>

</xml_diff>